<commit_message>
Possible fix for #15.
</commit_message>
<xml_diff>
--- a/examples/test_copy.xlsx
+++ b/examples/test_copy.xlsx
@@ -39,6 +39,9 @@
     <t>3:37 AM</t>
   </si>
   <si>
+    <t>nothing</t>
+  </si>
+  <si>
     <t>key</t>
   </si>
   <si>
@@ -63,6 +66,9 @@
     <t>This content goes to 12</t>
   </si>
   <si>
+    <t>nothing</t>
+  </si>
+  <si>
     <t>term</t>
   </si>
   <si>
@@ -85,6 +91,9 @@
   </si>
   <si>
     <t>What kind?</t>
+  </si>
+  <si>
+    <t>nothing</t>
   </si>
 </sst>
 </file>
@@ -199,6 +208,9 @@
       </c>
     </row>
     <row r="5">
+      <c t="s" s="1" r="A5">
+        <v>8</v>
+      </c>
       <c s="3" r="B5"/>
     </row>
     <row r="6">
@@ -3200,34 +3212,39 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>15</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5">
+      <c t="s" s="1" r="A5">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -3244,34 +3261,39 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>23</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5">
+      <c t="s" s="1" r="A5">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed json handling of rows with keys but no values
</commit_message>
<xml_diff>
--- a/examples/test_copy.xlsx
+++ b/examples/test_copy.xlsx
@@ -6,6 +6,7 @@
     <sheet sheetId="1" name="attribution" state="visible" r:id="rId3"/>
     <sheet sheetId="2" name="content" state="visible" r:id="rId4"/>
     <sheet sheetId="3" name="example_list" state="visible" r:id="rId5"/>
+    <sheet sheetId="4" name="key_without_value" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -94,6 +95,33 @@
   </si>
   <si>
     <t>nothing</t>
+  </si>
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>name </t>
+  </si>
+  <si>
+    <t>bio</t>
+  </si>
+  <si>
+    <t>first-last</t>
+  </si>
+  <si>
+    <t>first last</t>
+  </si>
+  <si>
+    <t>foo</t>
+  </si>
+  <si>
+    <t>hi-lo</t>
+  </si>
+  <si>
+    <t>hi lo</t>
+  </si>
+  <si>
+    <t>boo</t>
   </si>
 </sst>
 </file>
@@ -168,6 +196,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
@@ -3299,4 +3331,50 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c t="s" s="1" r="A1">
+        <v>27</v>
+      </c>
+      <c t="s" s="1" r="B1">
+        <v>28</v>
+      </c>
+      <c t="s" s="1" r="C1">
+        <v>29</v>
+      </c>
+      <c s="1" r="D1"/>
+    </row>
+    <row r="2">
+      <c t="s" s="1" r="A2">
+        <v>30</v>
+      </c>
+      <c t="s" s="1" r="B2">
+        <v>31</v>
+      </c>
+      <c t="s" s="1" r="C2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3">
+      <c t="s" s="1" r="A3">
+        <v>33</v>
+      </c>
+      <c t="s" s="1" r="B3">
+        <v>34</v>
+      </c>
+      <c t="s" s="1" r="C3">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>